<commit_message>
test change type date to instant 5f905a78062ed80c786d358f7097627c9896c9c1
</commit_message>
<xml_diff>
--- a/ig/eclairereviewdate-change-type-instant/StructureDefinition-eclaire-review-date.xlsx
+++ b/ig/eclairereviewdate-change-type-instant/StructureDefinition-eclaire-review-date.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-08-23T12:20:42+00:00</t>
+    <t>2023-08-23T12:56:18+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -211,7 +211,7 @@
     <t>Extension.value[x]</t>
   </si>
   <si>
-    <t xml:space="preserve">date
+    <t xml:space="preserve">instant
 </t>
   </si>
   <si>

</xml_diff>